<commit_message>
Added menu for langage selection. Moved message logging to it's own class. Logging for tag parser.
</commit_message>
<xml_diff>
--- a/Presets.xlsx
+++ b/Presets.xlsx
@@ -8,36 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projects\TIA_API\TIAEKtool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3B2CC069-86AB-4C78-AC66-8EE15570032A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD63046-9DB8-4119-B28A-ED4762347B39}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18615" windowHeight="10290" xr2:uid="{E0DF1621-78EA-4977-BC9C-C9EEE691EC86}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22605" windowHeight="10290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179021"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr dataExtractLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>falsk</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -69,54 +68,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="1">
     <dxf>
       <font>
-        <strike val="0"/>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.24994659260841701"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </font>
     </dxf>
   </dxfs>
@@ -130,82 +85,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$B$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>171449</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>0</xdr:col>
-          <xdr:colOff>266700</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>28575</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Check Box 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B14E78E2-41CF-4A44-B87C-72F0042DE1A2}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -504,19 +383,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8892BAB9-2978-4490-877B-34F875B8FF04}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0000-0000-0000-000000000000}">
   <dimension ref="B7:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C7" t="b">
@@ -524,7 +398,7 @@
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="b">
+      <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C8">
@@ -544,74 +418,17 @@
       <c r="B12" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C8">
-    <cfRule type="expression" dxfId="8" priority="23">
-      <formula>B8</formula>
+  <conditionalFormatting sqref="B9">
+    <cfRule type="expression" priority="2">
+      <formula>$B$8</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="7" priority="17">
-      <formula>B11</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="18">
-      <formula>B11='TRUE'</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="5" priority="15">
-      <formula>B12</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="16">
-      <formula>B12='TRUE'</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>B9</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>B9='TRUE'</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>B10</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
-      <formula>B10='TRUE'</formula>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$B$8</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x14">
-      <controls>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1025" r:id="rId4" name="Check Box 1">
-              <controlPr locked="0" defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>0</xdr:col>
-                    <xdr:colOff>266700</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>28575</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-      </controls>
-    </mc:Choice>
-  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>